<commit_message>
add test result details
</commit_message>
<xml_diff>
--- a/开奖测试/TestingResults.xlsx
+++ b/开奖测试/TestingResults.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>PlayerNumber</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,10 +101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Modified Rules</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hash</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -137,6 +133,10 @@
     <t>33aa399ee7e4765df67b06b15e7bf148894b043b1e121d8de296215b2f81cc1d</t>
   </si>
   <si>
+    <t>100X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>10X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -150,6 +150,60 @@
   </si>
   <si>
     <t>706d04845186fd385d8eb6c0ec940dba9a9145d45dafe6eee507c908411fec4f</t>
+  </si>
+  <si>
+    <t>2018-11-6-16-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>withour Mag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with Mag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018-11-6-16-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65fe300b17218df296a42cad2c9becf49f8bba202bf916df3e7a9cdbd52392c8</t>
+  </si>
+  <si>
+    <t>772d4ef759cb152600d5e17ce4bca53cad609fbe44bf742142b75ecba58dda50</t>
+  </si>
+  <si>
+    <t>Modified Rules Below</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018-11-7-10-36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e11f3eee0d1f1bb5b9f9353ad8cf97a7d4db36a558220409d4cf3590178ee18f</t>
+  </si>
+  <si>
+    <t>07c7d671713236d3de5dad396c29631d4089a4ff868c94ff61a9276d62a55b71</t>
+  </si>
+  <si>
+    <t>2018-11-7-11-15</t>
+  </si>
+  <si>
+    <t>Error, time eror</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018-11-7-11-18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>295a485642cf7dfa9a61f223b4773c16b19a908f268530ea3a00c3f8cbd1c866</t>
   </si>
 </sst>
 </file>
@@ -181,12 +235,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -201,12 +261,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -489,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -502,7 +565,7 @@
     <col min="3" max="4" width="14" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="65.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="60.21875" style="1" customWidth="1"/>
     <col min="8" max="8" width="40.21875" style="1" customWidth="1"/>
     <col min="9" max="11" width="11.109375" style="1" customWidth="1"/>
     <col min="12" max="13" width="11.6640625" style="1" customWidth="1"/>
@@ -522,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -531,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>17</v>
@@ -548,7 +611,7 @@
         <v>202</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1">
         <v>5860</v>
@@ -568,7 +631,7 @@
         <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1">
         <v>2020</v>
@@ -588,7 +651,7 @@
         <v>1000</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1">
         <v>57220</v>
@@ -611,7 +674,7 @@
         <v>500</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1">
         <v>9820</v>
@@ -634,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1">
         <v>20</v>
@@ -654,7 +717,7 @@
         <v>500</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1">
         <v>10000</v>
@@ -674,7 +737,7 @@
         <v>1000</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1">
         <v>20000</v>
@@ -694,7 +757,7 @@
         <v>1000</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="1">
         <v>20000</v>
@@ -706,35 +769,35 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B11" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="C11" s="3">
         <v>10</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="D11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="3">
         <v>1000</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>2.57275E-2</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>20</v>
+      <c r="G11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
         <v>100000000</v>
@@ -752,12 +815,12 @@
         <v>7.4352500000000002E-2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1">
         <v>100000000</v>
@@ -766,7 +829,7 @@
         <v>500</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1">
         <v>50000</v>
@@ -775,7 +838,7 @@
         <v>0.29124749999999999</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,6 +862,121 @@
       </c>
       <c r="G14" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1">
+        <v>100</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2.0312500000000001E-2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1">
+        <v>100</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.0400499999999998E-2</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.51731349999999998</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1">
+        <v>200</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1">
+        <v>200</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.49364249999999998</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>